<commit_message>
working towards final notebook
</commit_message>
<xml_diff>
--- a/descriptions_top_factors.xlsx
+++ b/descriptions_top_factors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aosika\flatiron-ds-course\mod3_v21\dsc-mod-3-project-v2-1-online-ds-pt-100719\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F30B27-2813-48EA-8F24-C9711E40F3E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0E17AF-5FDA-4850-9E7A-0E55D7EDE28A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B19CAB33-3DCD-4CB4-89E0-7CEC37E1F7F6}"/>
   </bookViews>
@@ -31,28 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
-  <si>
-    <t>Feature:</t>
-  </si>
-  <si>
-    <t>Exhibiting COVID-19 symptoms</t>
-  </si>
-  <si>
-    <t>Belief in contracting the disease</t>
-  </si>
-  <si>
-    <t>Household practiced social distancing &amp; hygiene</t>
-  </si>
-  <si>
-    <t>Taking prescription medication</t>
-  </si>
-  <si>
-    <t>Travel</t>
-  </si>
-  <si>
-    <t>Correlation:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>+</t>
   </si>
@@ -60,20 +39,65 @@
     <t>-</t>
   </si>
   <si>
-    <t>Contact with others infected with COVID-19</t>
-  </si>
-  <si>
-    <t>Individual practiced social distancing &amp; hygiene</t>
-  </si>
-  <si>
     <t>Importance</t>
+  </si>
+  <si>
+    <t>opinion_infection</t>
+  </si>
+  <si>
+    <t>covid19_symptoms</t>
+  </si>
+  <si>
+    <t>covid19_contact</t>
+  </si>
+  <si>
+    <t>rate_reducing_risk_house</t>
+  </si>
+  <si>
+    <t>omwasnull</t>
+  </si>
+  <si>
+    <t>rate_reducing_risk_single</t>
+  </si>
+  <si>
+    <t>oiwasnull</t>
+  </si>
+  <si>
+    <t>sex_male</t>
+  </si>
+  <si>
+    <t>sex_female</t>
+  </si>
+  <si>
+    <t>bmi</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taking_prescription_medication	</t>
+  </si>
+  <si>
+    <t>Opinion Infection was left null</t>
+  </si>
+  <si>
+    <t>Individual was in contact with another who was COVID-19 +</t>
+  </si>
+  <si>
+    <t>Individual exhibited COVID-19 symptops</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,24 +112,19 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="26"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="18"/>
+      <sz val="6"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +140,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -152,29 +177,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,91 +506,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD18D433-5159-4A3B-B6D8-C2B15FB92ED9}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.6328125" customWidth="1"/>
-    <col min="2" max="3" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="67.81640625" customWidth="1"/>
+    <col min="2" max="2" width="52.26953125" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="38.5" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" ht="38.5" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="33.5" x14ac:dyDescent="0.75">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2">
+        <v>0.52973499999999996</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.28541499999999997</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="33.5" x14ac:dyDescent="0.75">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.122519</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="33.5" x14ac:dyDescent="0.75">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1">
+        <v>1.36553E-2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="33.5" x14ac:dyDescent="0.75">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2">
+        <v>1.27974E-2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="33.5" x14ac:dyDescent="0.75">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="1">
+        <v>1.08048E-2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="33.5" x14ac:dyDescent="0.75">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7.3136700000000004E-3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="33.5" x14ac:dyDescent="0.75">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1">
+        <v>6.41232E-3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="33.5" x14ac:dyDescent="0.75">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="1" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2">
+        <v>3.5449100000000001E-3</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="33.5" x14ac:dyDescent="0.75">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="49" x14ac:dyDescent="0.75">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" ht="33.5" x14ac:dyDescent="0.75">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="33.5" x14ac:dyDescent="0.75">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" ht="49" x14ac:dyDescent="0.75">
-      <c r="A8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="33.5" x14ac:dyDescent="0.75">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1">
+        <v>2.4780599999999998E-3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="67" x14ac:dyDescent="0.75">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2">
+        <v>3.5449100000000001E-3</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>